<commit_message>
Terminado TPP y faltan graficas algoritmia
</commit_message>
<xml_diff>
--- a/Algoritmia/Practica/Entrega 3/Algoritmos.xlsx
+++ b/Algoritmia/Practica/Entrega 3/Algoritmos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blanc\OneDrive\Documentos\2-curso-2-cuatri\Algoritmia\Practica\Entrega 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152FDBD6-087F-4176-95CB-040888E942E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AF37B0-1D87-455E-93A4-4684F1F1EFFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10395" yWindow="7800" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="36">
   <si>
     <t>Substracción 1</t>
   </si>
@@ -49,12 +49,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>t(ms)</t>
-  </si>
-  <si>
-    <t>t teórico(ms)</t>
-  </si>
-  <si>
     <t>Substracción 2</t>
   </si>
   <si>
@@ -101,13 +95,61 @@
   </si>
   <si>
     <t>División 4</t>
+  </si>
+  <si>
+    <t>Fibonacci 1</t>
+  </si>
+  <si>
+    <t>nVeces=10e9</t>
+  </si>
+  <si>
+    <t>t(ns)</t>
+  </si>
+  <si>
+    <t>bastante semejante</t>
+  </si>
+  <si>
+    <t>t teórico(ns)</t>
+  </si>
+  <si>
+    <t>t(ps)</t>
+  </si>
+  <si>
+    <t>picosegundos</t>
+  </si>
+  <si>
+    <t>t teórico(ps)</t>
+  </si>
+  <si>
+    <t>Fibonacci 2</t>
+  </si>
+  <si>
+    <t>Fibonacci 3</t>
+  </si>
+  <si>
+    <t>Fibonacci 4</t>
+  </si>
+  <si>
+    <t>Complejidad= O(1.6^n)</t>
+  </si>
+  <si>
+    <t>VectorSum 1</t>
+  </si>
+  <si>
+    <t>se parece mucho</t>
+  </si>
+  <si>
+    <t>VectorSum 2</t>
+  </si>
+  <si>
+    <t>VectorSum 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,8 +157,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,8 +179,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -153,11 +221,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -167,10 +257,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -487,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="F142" sqref="F142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,20 +615,20 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -581,25 +690,25 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="5"/>
+      <c r="C10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -659,30 +768,30 @@
         <v>357798.2109375</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="5"/>
+      <c r="C19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -778,30 +887,30 @@
         <v>219395.625</v>
       </c>
       <c r="D28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="5"/>
+      <c r="C31" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -862,26 +971,26 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" s="1" t="s">
+      <c r="A40" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" s="5"/>
+      <c r="C40" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -954,26 +1063,26 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50" s="1" t="s">
+      <c r="A50" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D50" s="5"/>
+      <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1045,30 +1154,30 @@
         <v>27086</v>
       </c>
       <c r="D57" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60" s="5"/>
+      <c r="C60" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="6"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1088,7 +1197,7 @@
         <v>17898</v>
       </c>
       <c r="C63" s="3">
-        <f t="shared" ref="C63:C69" si="1">($A63/$A62)*$B62</f>
+        <f t="shared" ref="C63:C66" si="1">($A63/$A62)*$B62</f>
         <v>2689.2307692307695</v>
       </c>
     </row>
@@ -1104,7 +1213,7 @@
         <v>21253.875</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>22</v>
       </c>
@@ -1116,7 +1225,7 @@
         <v>185352.31578947368</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>25</v>
       </c>
@@ -1128,43 +1237,43 @@
         <v>196573.86363636365</v>
       </c>
       <c r="D66" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B69" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D69" s="5"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" s="10"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>8</v>
       </c>
@@ -1173,7 +1282,7 @@
       </c>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>16</v>
       </c>
@@ -1185,7 +1294,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>32</v>
       </c>
@@ -1197,7 +1306,7 @@
         <v>2616</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>64</v>
       </c>
@@ -1209,7 +1318,7 @@
         <v>22252</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>128</v>
       </c>
@@ -1221,7 +1330,7 @@
         <v>44486</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>256</v>
       </c>
@@ -1233,11 +1342,662 @@
         <v>347870</v>
       </c>
       <c r="D76" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" s="8"/>
+      <c r="E79" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="3">
+        <v>10</v>
+      </c>
+      <c r="B81" s="3">
+        <v>3402</v>
+      </c>
+      <c r="C81" s="3"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
+        <v>11</v>
+      </c>
+      <c r="B82" s="3">
+        <v>4301</v>
+      </c>
+      <c r="C82" s="3">
+        <f>($A82/$A81)*$B81</f>
+        <v>3742.2000000000003</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <v>12</v>
+      </c>
+      <c r="B83" s="3">
+        <v>5246</v>
+      </c>
+      <c r="C83" s="3">
+        <f>($A83/$A82)*$B82</f>
+        <v>4692</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <v>13</v>
+      </c>
+      <c r="B84" s="3">
+        <v>5369</v>
+      </c>
+      <c r="C84" s="3">
+        <f>($A84/$A83)*$B83</f>
+        <v>5683.1666666666661</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
+        <v>14</v>
+      </c>
+      <c r="B85" s="3">
+        <v>6154</v>
+      </c>
+      <c r="C85" s="3">
+        <f>($A85/$A84)*$B84</f>
+        <v>5782</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
+        <v>15</v>
+      </c>
+      <c r="B86" s="3">
+        <v>6282</v>
+      </c>
+      <c r="C86" s="3">
+        <f>($A86/$A85)*$B85</f>
+        <v>6593.5714285714284</v>
+      </c>
+      <c r="D86" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" s="8"/>
+      <c r="E89" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
+        <v>10</v>
+      </c>
+      <c r="B91" s="3">
+        <v>5090</v>
+      </c>
+      <c r="C91" s="3"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
+        <v>11</v>
+      </c>
+      <c r="B92" s="3">
+        <v>6865</v>
+      </c>
+      <c r="C92" s="3">
+        <f>($A92/$A91)*$B91</f>
+        <v>5599</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
+        <v>12</v>
+      </c>
+      <c r="B93" s="3">
+        <v>7112</v>
+      </c>
+      <c r="C93" s="3">
+        <f>($A93/$A92)*$B92</f>
+        <v>7489.0909090909081</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="3">
+        <v>13</v>
+      </c>
+      <c r="B94" s="3">
+        <v>7988</v>
+      </c>
+      <c r="C94" s="3">
+        <f>($A94/$A93)*$B93</f>
+        <v>7704.6666666666661</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="3">
+        <v>14</v>
+      </c>
+      <c r="B95" s="3">
+        <v>7680</v>
+      </c>
+      <c r="C95" s="3">
+        <f>($A95/$A94)*$B94</f>
+        <v>8602.4615384615372</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="3">
+        <v>15</v>
+      </c>
+      <c r="B96" s="3">
+        <v>8227</v>
+      </c>
+      <c r="C96" s="3">
+        <f>($A96/$A95)*$B95</f>
+        <v>8228.5714285714275</v>
+      </c>
+      <c r="D96" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" s="8"/>
+      <c r="E99" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="3">
+        <v>10</v>
+      </c>
+      <c r="B101" s="3">
+        <v>10048</v>
+      </c>
+      <c r="C101" s="3"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="3">
+        <v>11</v>
+      </c>
+      <c r="B102" s="3">
+        <v>10468</v>
+      </c>
+      <c r="C102" s="3">
+        <f>($A102/$A101)*$B101</f>
+        <v>11052.800000000001</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="3">
+        <v>12</v>
+      </c>
+      <c r="B103" s="3">
+        <v>11001</v>
+      </c>
+      <c r="C103" s="3">
+        <f>($A103/$A102)*$B102</f>
+        <v>11419.636363636362</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="3">
+        <v>13</v>
+      </c>
+      <c r="B104" s="3">
+        <v>11213</v>
+      </c>
+      <c r="C104" s="3">
+        <f>($A104/$A103)*$B103</f>
+        <v>11917.75</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="3">
+        <v>14</v>
+      </c>
+      <c r="B105" s="3">
+        <v>12845</v>
+      </c>
+      <c r="C105" s="3">
+        <f>($A105/$A104)*$B104</f>
+        <v>12075.538461538461</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="3">
+        <v>15</v>
+      </c>
+      <c r="B106" s="3">
+        <v>13516</v>
+      </c>
+      <c r="C106" s="3">
+        <f>($A106/$A105)*$B105</f>
+        <v>13762.5</v>
+      </c>
+      <c r="D106" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D109" s="8"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="3">
+        <v>13</v>
+      </c>
+      <c r="B111" s="3">
+        <v>985</v>
+      </c>
+      <c r="C111" s="3"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="3">
+        <v>14</v>
+      </c>
+      <c r="B112" s="3">
+        <v>1631</v>
+      </c>
+      <c r="C112" s="3">
+        <f>($A112/$A111)*$B111</f>
+        <v>1060.7692307692307</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="3">
+        <v>15</v>
+      </c>
+      <c r="B113" s="3">
+        <v>2596</v>
+      </c>
+      <c r="C113" s="3">
+        <f>($A113/$A112)*$B112</f>
+        <v>1747.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="3">
+        <v>16</v>
+      </c>
+      <c r="B114" s="3">
+        <v>3766</v>
+      </c>
+      <c r="C114" s="3">
+        <f>($A114/$A113)*$B113</f>
+        <v>2769.0666666666666</v>
+      </c>
+      <c r="F114" s="11"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="3">
+        <v>17</v>
+      </c>
+      <c r="B115" s="3">
+        <v>6744</v>
+      </c>
+      <c r="C115" s="3">
+        <f>($A115/$A114)*$B114</f>
+        <v>4001.375</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="3">
+        <v>18</v>
+      </c>
+      <c r="B116" s="3">
+        <v>10311</v>
+      </c>
+      <c r="C116" s="3">
+        <f>($A116/$A115)*$B115</f>
+        <v>7140.7058823529414</v>
+      </c>
+      <c r="D116" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B119" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D119" s="13"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="3">
+        <v>3072</v>
+      </c>
+      <c r="B121" s="3">
+        <v>1031</v>
+      </c>
+      <c r="C121" s="3"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="3">
+        <v>6144</v>
+      </c>
+      <c r="B122" s="3">
+        <v>1951</v>
+      </c>
+      <c r="C122" s="3">
+        <f>($A122/$A121)*$B121</f>
+        <v>2062</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="3">
+        <v>12288</v>
+      </c>
+      <c r="B123" s="3">
+        <v>4420</v>
+      </c>
+      <c r="C123" s="3">
+        <f>($A123/$A122)*$B122</f>
+        <v>3902</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="3">
+        <v>24576</v>
+      </c>
+      <c r="B124" s="3">
+        <v>8078</v>
+      </c>
+      <c r="C124" s="3">
+        <f>($A124/$A123)*$B123</f>
+        <v>8840</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="14">
+        <v>49152</v>
+      </c>
+      <c r="B125" s="14">
+        <v>16397</v>
+      </c>
+      <c r="C125" s="14">
+        <f>($A125/$A124)*$B124</f>
+        <v>16156</v>
+      </c>
+      <c r="D125" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="15"/>
+      <c r="B126" s="15"/>
+      <c r="C126" s="15"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B128" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C128" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D128" s="13"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="3">
+        <v>768</v>
+      </c>
+      <c r="B130" s="3">
+        <v>3124</v>
+      </c>
+      <c r="C130" s="3"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="3">
+        <v>1536</v>
+      </c>
+      <c r="B131" s="3">
+        <v>6467</v>
+      </c>
+      <c r="C131" s="3">
+        <f>($A131/$A130)*$B130</f>
+        <v>6248</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="3">
+        <v>3072</v>
+      </c>
+      <c r="B132" s="3">
+        <v>14192</v>
+      </c>
+      <c r="C132" s="3">
+        <f>($A132/$A131)*$B131</f>
+        <v>12934</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="3">
+        <v>6144</v>
+      </c>
+      <c r="B133" s="3">
+        <v>28809</v>
+      </c>
+      <c r="C133" s="3">
+        <f>($A133/$A132)*$B132</f>
+        <v>28384</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="3">
+        <v>12288</v>
+      </c>
+      <c r="B134" s="3">
+        <v>58721</v>
+      </c>
+      <c r="C134" s="3">
+        <f>($A134/$A133)*$B133</f>
+        <v>57618</v>
+      </c>
+      <c r="D134" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B136" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D136" s="13"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="3">
+        <v>384</v>
+      </c>
+      <c r="B138" s="3">
+        <v>1129</v>
+      </c>
+      <c r="C138" s="3"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="3">
+        <v>768</v>
+      </c>
+      <c r="B139" s="3">
+        <v>2546</v>
+      </c>
+      <c r="C139" s="3">
+        <f>($A139/$A138)*$B138</f>
+        <v>2258</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="3">
+        <v>1536</v>
+      </c>
+      <c r="B140" s="3">
+        <v>4613</v>
+      </c>
+      <c r="C140" s="3">
+        <f>($A140/$A139)*$B139</f>
+        <v>5092</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="3">
+        <v>3072</v>
+      </c>
+      <c r="B141" s="3">
+        <v>10713</v>
+      </c>
+      <c r="C141" s="3">
+        <f>($A141/$A140)*$B140</f>
+        <v>9226</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="3">
+        <v>6144</v>
+      </c>
+      <c r="B142" s="3">
+        <v>19433</v>
+      </c>
+      <c r="C142" s="3">
+        <f>($A142/$A141)*$B141</f>
+        <v>21426</v>
+      </c>
+      <c r="D142" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="15">
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C136:D136"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C119:D119"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="C60:D60"/>
     <mergeCell ref="C69:D69"/>
@@ -1248,5 +2008,6 @@
     <mergeCell ref="C40:D40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>